<commit_message>
Arreglo de plusvalias de comunas :zap:
</commit_message>
<xml_diff>
--- a/db/Plusvalias/Region Metropolitana.xlsx
+++ b/db/Plusvalias/Region Metropolitana.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moises/Desktop/depto2/db/Plusvalias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA748A5-1746-6840-B75F-80827B5B9523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D638DB-041F-B64E-8896-A10391AAF531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="2" xr2:uid="{3812CA6F-1638-0644-A936-18470B6A076E}"/>
+    <workbookView xWindow="33200" yWindow="1720" windowWidth="28040" windowHeight="16000" activeTab="4" xr2:uid="{3812CA6F-1638-0644-A936-18470B6A076E}"/>
   </bookViews>
   <sheets>
     <sheet name="La Florida" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="La Cisterna" sheetId="7" r:id="rId4"/>
     <sheet name="Santiago" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,47 +40,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="29">
   <si>
     <t>UF/m2</t>
   </si>
   <si>
-    <t>1S 2012</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>2S 2012</t>
-  </si>
-  <si>
-    <t>1S 2013</t>
-  </si>
-  <si>
-    <t>2S 2013</t>
-  </si>
-  <si>
-    <t>1S 2014</t>
-  </si>
-  <si>
-    <t>2S 2014</t>
-  </si>
-  <si>
-    <t>1S 2015</t>
-  </si>
-  <si>
-    <t>2S 2015</t>
-  </si>
-  <si>
-    <t>1S 2016</t>
-  </si>
-  <si>
-    <t>2S 2016</t>
-  </si>
-  <si>
-    <t>1S 2017</t>
-  </si>
-  <si>
     <t>2S 2017</t>
   </si>
   <si>
@@ -121,39 +88,6 @@
   </si>
   <si>
     <t>Semestre</t>
-  </si>
-  <si>
-    <t>1S2012</t>
-  </si>
-  <si>
-    <t>2S2012</t>
-  </si>
-  <si>
-    <t>1S2013</t>
-  </si>
-  <si>
-    <t>2S2013</t>
-  </si>
-  <si>
-    <t>1S2014</t>
-  </si>
-  <si>
-    <t>2S2014</t>
-  </si>
-  <si>
-    <t>1S2015</t>
-  </si>
-  <si>
-    <t>2S2015</t>
-  </si>
-  <si>
-    <t>1S2016</t>
-  </si>
-  <si>
-    <t>2S2016</t>
-  </si>
-  <si>
-    <t>1S2017</t>
   </si>
   <si>
     <t>2S2017</t>
@@ -199,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,6 +154,13 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -238,16 +179,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -582,14 +526,14 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="A15" sqref="A15:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -597,195 +541,151 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2">
-        <v>32.1</v>
+        <v>48.9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2">
-        <v>32.4</v>
+        <v>50.9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2">
-        <v>32.700000000000003</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2">
-        <v>35.9</v>
+        <v>55.3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
-        <v>35.6</v>
+        <v>60.6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>41.1</v>
+        <v>59.8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2">
-        <v>42.7</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2">
-        <v>41.9</v>
+        <v>64.3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2">
-        <v>45.1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2">
-        <v>45</v>
+        <v>70.8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2">
-        <v>47.9</v>
+        <v>73.2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2">
-        <v>48.9</v>
+        <v>73.3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2">
-        <v>50.9</v>
+        <v>75.3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="2">
-        <v>53</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="2">
-        <v>55.3</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="2">
-        <v>60.6</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="2">
-        <v>59.8</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="2">
-        <v>62.6</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="2">
-        <v>64.3</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="2">
-        <v>68</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="2">
-        <v>70.8</v>
-      </c>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="2">
-        <v>73.2</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="2">
-        <v>73.3</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="2">
-        <v>75.3</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -794,17 +694,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738CE7E5-E6C9-A749-B2B2-5BF05B17017E}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="A2" sqref="A2:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -812,10 +712,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>30.3</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -823,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>36.1</v>
+        <v>59.2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -831,7 +731,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>37.200000000000003</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -839,7 +739,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>39.799999999999997</v>
+        <v>61.2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -847,7 +747,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>42.1</v>
+        <v>66.7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -855,7 +755,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>44.3</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -863,7 +763,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>45.1</v>
+        <v>66.599999999999994</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -871,7 +771,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>46</v>
+        <v>70.400000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -879,7 +779,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>48.4</v>
+        <v>74.8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -887,7 +787,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>47.2</v>
+        <v>74.5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -895,7 +795,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>49.1</v>
+        <v>76.599999999999994</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -903,103 +803,15 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>57</v>
+        <v>78.2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2">
-        <v>59.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
-        <v>61.2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2">
-        <v>66.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2">
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2">
-        <v>66.599999999999994</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2">
-        <v>70.400000000000006</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2">
-        <v>74.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="2">
-        <v>74.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="2">
-        <v>76.599999999999994</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="2">
-        <v>78.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>2</v>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1011,15 +823,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAA178E-901E-6745-AF5D-A52FAC6FC1DE}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1027,10 +839,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>41.1</v>
+        <v>75.900000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1038,7 +850,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>48.7</v>
+        <v>76.599999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1046,7 +858,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>49</v>
+        <v>79.8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1054,7 +866,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>50.6</v>
+        <v>81.7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1062,7 +874,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>57.6</v>
+        <v>81.7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1070,7 +882,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>60.6</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1078,7 +890,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>64.099999999999994</v>
+        <v>82.7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1086,7 +898,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>67.5</v>
+        <v>86.3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1094,7 +906,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>68.7</v>
+        <v>88.8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1102,7 +914,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>69</v>
+        <v>90.2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1110,7 +922,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>70.8</v>
+        <v>85.8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1118,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>75.900000000000006</v>
+        <v>88.4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1126,96 +938,52 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>76.599999999999994</v>
+        <v>91.1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2">
-        <v>79.8</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
-        <v>81.7</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2">
-        <v>81.7</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2">
-        <v>82</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2">
-        <v>82.7</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2">
-        <v>86.3</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2">
-        <v>88.8</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="2">
-        <v>90.2</v>
-      </c>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="2">
-        <v>85.8</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="2">
-        <v>88.4</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="2">
-        <v>91.1</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1224,17 +992,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F530C9-A0A3-9248-BD09-66CE33776A04}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B25"/>
+      <selection activeCell="A2" sqref="A2:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1242,10 +1010,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45.9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1253,7 +1021,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>27.6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1261,7 +1029,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>27.5</v>
+        <v>54.2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1269,7 +1037,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>29.9</v>
+        <v>53.3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1277,7 +1045,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>32.200000000000003</v>
+        <v>56.8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1285,7 +1053,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>35</v>
+        <v>57.8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1293,7 +1061,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>35.700000000000003</v>
+        <v>59.4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1301,7 +1069,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>36</v>
+        <v>60.6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1309,7 +1077,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>38.799999999999997</v>
+        <v>63.6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1317,7 +1085,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>40.200000000000003</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1325,7 +1093,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>43.1</v>
+        <v>64.900000000000006</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1333,103 +1101,15 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>45.9</v>
+        <v>65.400000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2">
-        <v>54.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
-        <v>53.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2">
-        <v>56.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2">
-        <v>57.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2">
-        <v>59.4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2">
-        <v>60.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2">
-        <v>63.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="2">
-        <v>63.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="2">
-        <v>64.900000000000006</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="2">
-        <v>65.400000000000006</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>2</v>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1439,17 +1119,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C684211-31D3-134C-B84F-B00211A830ED}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1457,10 +1137,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>35.9</v>
+        <v>60.2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1468,7 +1148,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>39.4</v>
+        <v>62.2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1476,7 +1156,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>40.6</v>
+        <v>66.900000000000006</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1484,7 +1164,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>45.3</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1492,7 +1172,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>46.6</v>
+        <v>74.8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1500,7 +1180,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>50.8</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1508,7 +1188,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>53.2</v>
+        <v>74.7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1516,7 +1196,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>54.7</v>
+        <v>74.599999999999994</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1524,7 +1204,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>56.3</v>
+        <v>76.900000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1532,7 +1212,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>57.8</v>
+        <v>77.7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1540,7 +1220,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>56.5</v>
+        <v>79.099999999999994</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1548,7 +1228,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>60.2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1556,96 +1236,12 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>62.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2">
-        <v>66.900000000000006</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2">
-        <v>74.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2">
-        <v>73.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2">
-        <v>74.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2">
-        <v>74.599999999999994</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2">
-        <v>76.900000000000006</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="2">
-        <v>77.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="2">
-        <v>79.099999999999994</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="2">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="2">
         <v>81.2</v>
       </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>